<commit_message>
Updated marks, output file, and script logic
</commit_message>
<xml_diff>
--- a/formatted_marks.xlsx
+++ b/formatted_marks.xlsx
@@ -432,10 +432,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -619,6 +619,30 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Janifer</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>23</v>
+      </c>
+      <c r="C8" t="n">
+        <v>45</v>
+      </c>
+      <c r="D8" t="n">
+        <v>53</v>
+      </c>
+      <c r="E8" t="n">
+        <v>121</v>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>